<commit_message>
Final updates for revisions
In EDC 1:
Changed map water from blue to white to match journal specifications. Updated ggtext colors to match region colors in other figures.

In EDC 5:
Updated fig 3 to resolve gridline non-matching issue (specified scale limits to resolve).

Added a ggsave line to create PDF versions of all main text figures for publication.
</commit_message>
<xml_diff>
--- a/figures_tables/Formatted Tables.xlsx
+++ b/figures_tables/Formatted Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahrempel/My Drive/Research_Archives/ecological_drivers_corallivory/figures_tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37074A17-0225-C54A-8F69-EA817A171388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E63B8CE-B1FA-8542-85F4-45D7A7296A99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41840" yWindow="500" windowWidth="24360" windowHeight="19240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="55160" yWindow="500" windowWidth="24360" windowHeight="19240" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="14" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="186">
   <si>
     <t>Region</t>
   </si>
@@ -871,6 +871,18 @@
       </rPr>
       <t>)</t>
     </r>
+  </si>
+  <si>
+    <t>[-7.549, -3.352]</t>
+  </si>
+  <si>
+    <t>[0.007, 0.122]</t>
+  </si>
+  <si>
+    <t>[-0.191, 0.035]</t>
+  </si>
+  <si>
+    <t>[-0.003, 0.005]</t>
   </si>
 </sst>
 </file>
@@ -1772,6 +1784,126 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="36" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="37" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="37" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="38" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="38" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="22" fillId="39" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="22" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="39" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="44" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="44" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="22" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="22" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1780,126 +1912,6 @@
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="36" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="37" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="37" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="38" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="38" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="22" fillId="39" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="22" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="39" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="44" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="44" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="22" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="22" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -2264,7 +2276,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FCC5641-2513-5944-B608-C8258FEA94F5}">
   <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="185" workbookViewId="0">
+    <sheetView zoomScale="185" workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
@@ -2290,100 +2302,100 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="97" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="100" t="s">
+      <c r="B1" s="95" t="s">
         <v>181</v>
       </c>
-      <c r="C1" s="100"/>
-      <c r="D1" s="100"/>
-      <c r="E1" s="100" t="s">
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
+      <c r="E1" s="95" t="s">
         <v>70</v>
       </c>
-      <c r="F1" s="100"/>
-      <c r="G1" s="100"/>
-      <c r="H1" s="100" t="s">
+      <c r="F1" s="95"/>
+      <c r="G1" s="95"/>
+      <c r="H1" s="95" t="s">
         <v>180</v>
       </c>
-      <c r="I1" s="100"/>
-      <c r="J1" s="100"/>
-      <c r="K1" s="100" t="s">
+      <c r="I1" s="95"/>
+      <c r="J1" s="95"/>
+      <c r="K1" s="95" t="s">
         <v>179</v>
       </c>
-      <c r="L1" s="100"/>
-      <c r="M1" s="100"/>
-      <c r="N1" s="100" t="s">
+      <c r="L1" s="95"/>
+      <c r="M1" s="95"/>
+      <c r="N1" s="95" t="s">
         <v>178</v>
       </c>
-      <c r="O1" s="100"/>
-      <c r="P1" s="100"/>
+      <c r="O1" s="95"/>
+      <c r="P1" s="95"/>
     </row>
     <row r="2" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="99"/>
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="98"/>
-      <c r="J2" s="98"/>
-      <c r="K2" s="98"/>
-      <c r="L2" s="98"/>
-      <c r="M2" s="98"/>
-      <c r="N2" s="98"/>
-      <c r="O2" s="98"/>
-      <c r="P2" s="98"/>
+      <c r="A2" s="98"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="96"/>
+      <c r="J2" s="96"/>
+      <c r="K2" s="96"/>
+      <c r="L2" s="96"/>
+      <c r="M2" s="96"/>
+      <c r="N2" s="96"/>
+      <c r="O2" s="96"/>
+      <c r="P2" s="96"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="84">
+      <c r="B3" s="81">
         <v>0.8</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="D3" s="95">
+      <c r="D3" s="92">
         <v>0.4</v>
       </c>
-      <c r="E3" s="76">
+      <c r="E3" s="73">
         <v>18</v>
       </c>
-      <c r="F3" s="97" t="s">
+      <c r="F3" s="94" t="s">
         <v>177</v>
       </c>
-      <c r="G3" s="96">
+      <c r="G3" s="93">
         <v>3.7</v>
       </c>
-      <c r="H3" s="84">
+      <c r="H3" s="81">
         <v>0.9</v>
       </c>
       <c r="I3" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="J3" s="95">
+      <c r="J3" s="92">
         <v>0.2</v>
       </c>
-      <c r="K3" s="93">
+      <c r="K3" s="90">
         <v>0.33300000000000002</v>
       </c>
       <c r="L3" s="24" t="s">
         <v>177</v>
       </c>
-      <c r="M3" s="94">
+      <c r="M3" s="91">
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="N3" s="93">
+      <c r="N3" s="90">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="O3" s="24" t="s">
         <v>177</v>
       </c>
-      <c r="P3" s="92">
+      <c r="P3" s="89">
         <v>1E-3</v>
       </c>
     </row>
@@ -2391,49 +2403,49 @@
       <c r="A4" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="91">
+      <c r="B4" s="88">
         <v>3.9</v>
       </c>
-      <c r="C4" s="90" t="s">
+      <c r="C4" s="87" t="s">
         <v>177</v>
       </c>
-      <c r="D4" s="89">
+      <c r="D4" s="86">
         <v>1</v>
       </c>
-      <c r="E4" s="84">
+      <c r="E4" s="81">
         <v>2.8</v>
       </c>
       <c r="F4" s="24" t="s">
         <v>177</v>
       </c>
-      <c r="G4" s="72">
+      <c r="G4" s="69">
         <v>1.9</v>
       </c>
-      <c r="H4" s="88">
+      <c r="H4" s="85">
         <v>121.7</v>
       </c>
-      <c r="I4" s="83" t="s">
+      <c r="I4" s="80" t="s">
         <v>177</v>
       </c>
-      <c r="J4" s="82">
+      <c r="J4" s="79">
         <v>38.9</v>
       </c>
-      <c r="K4" s="87">
+      <c r="K4" s="84">
         <v>0.63</v>
       </c>
-      <c r="L4" s="86" t="s">
+      <c r="L4" s="83" t="s">
         <v>177</v>
       </c>
-      <c r="M4" s="85">
+      <c r="M4" s="82">
         <v>9.0999999999999998E-2</v>
       </c>
-      <c r="N4" s="84">
+      <c r="N4" s="81">
         <v>0.55300000000000005</v>
       </c>
-      <c r="O4" s="83" t="s">
+      <c r="O4" s="80" t="s">
         <v>177</v>
       </c>
-      <c r="P4" s="82">
+      <c r="P4" s="79">
         <v>0.14699999999999999</v>
       </c>
     </row>
@@ -2441,99 +2453,99 @@
       <c r="A5" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="79">
+      <c r="B5" s="76">
         <v>2.4</v>
       </c>
-      <c r="C5" s="81" t="s">
+      <c r="C5" s="78" t="s">
         <v>177</v>
       </c>
-      <c r="D5" s="80">
+      <c r="D5" s="77">
         <v>0.5</v>
       </c>
-      <c r="E5" s="79">
+      <c r="E5" s="76">
         <v>7.2</v>
       </c>
-      <c r="F5" s="78" t="s">
+      <c r="F5" s="75" t="s">
         <v>177</v>
       </c>
-      <c r="G5" s="77">
+      <c r="G5" s="74">
         <v>1.3</v>
       </c>
-      <c r="H5" s="76">
+      <c r="H5" s="73">
         <v>1.4</v>
       </c>
       <c r="I5" s="24" t="s">
         <v>177</v>
       </c>
-      <c r="J5" s="72">
+      <c r="J5" s="69">
         <v>0.7</v>
       </c>
-      <c r="K5" s="73">
+      <c r="K5" s="70">
         <v>1.17</v>
       </c>
-      <c r="L5" s="75" t="s">
+      <c r="L5" s="72" t="s">
         <v>177</v>
       </c>
-      <c r="M5" s="74">
+      <c r="M5" s="71">
         <v>0.44600000000000001</v>
       </c>
-      <c r="N5" s="73">
+      <c r="N5" s="70">
         <v>0.01</v>
       </c>
       <c r="O5" s="24" t="s">
         <v>177</v>
       </c>
-      <c r="P5" s="72">
+      <c r="P5" s="69">
         <v>2E-3</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A6" s="71" t="s">
+      <c r="A6" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="70">
+      <c r="B6" s="67">
         <v>7.6</v>
       </c>
-      <c r="C6" s="66" t="s">
+      <c r="C6" s="63" t="s">
         <v>177</v>
       </c>
-      <c r="D6" s="65">
+      <c r="D6" s="62">
         <v>0.5</v>
       </c>
-      <c r="E6" s="70">
+      <c r="E6" s="67">
         <v>23.3</v>
       </c>
-      <c r="F6" s="66" t="s">
+      <c r="F6" s="63" t="s">
         <v>177</v>
       </c>
-      <c r="G6" s="65">
+      <c r="G6" s="62">
         <v>4.0999999999999996</v>
       </c>
-      <c r="H6" s="69">
+      <c r="H6" s="66">
         <v>2</v>
       </c>
-      <c r="I6" s="68" t="s">
+      <c r="I6" s="65" t="s">
         <v>177</v>
       </c>
-      <c r="J6" s="67">
+      <c r="J6" s="64">
         <v>0.8</v>
       </c>
-      <c r="K6" s="64">
+      <c r="K6" s="61">
         <v>1.9930000000000001</v>
       </c>
-      <c r="L6" s="66" t="s">
+      <c r="L6" s="63" t="s">
         <v>177</v>
       </c>
-      <c r="M6" s="65">
+      <c r="M6" s="62">
         <v>0.79100000000000004</v>
       </c>
-      <c r="N6" s="64">
+      <c r="N6" s="61">
         <v>1.4E-2</v>
       </c>
-      <c r="O6" s="63" t="s">
+      <c r="O6" s="60" t="s">
         <v>177</v>
       </c>
-      <c r="P6" s="62">
+      <c r="P6" s="59">
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
@@ -2575,6 +2587,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E6">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </colorScale>
+    </cfRule>
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -2584,14 +2604,6 @@
       </colorScale>
     </cfRule>
     <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2609,7 +2621,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H6">
-    <cfRule type="colorScale" priority="12">
+    <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2617,7 +2629,7 @@
         <color theme="0" tint="-0.34998626667073579"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="13">
+    <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2627,7 +2639,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:K6">
-    <cfRule type="colorScale" priority="1">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2635,7 +2647,7 @@
         <color theme="0" tint="-0.34998626667073579"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="2">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2645,7 +2657,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3:N10">
-    <cfRule type="colorScale" priority="3">
+    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2653,7 +2665,7 @@
         <color theme="0" tint="-0.34998626667073579"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="4">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2689,34 +2701,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="99" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="99" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="59" t="s">
+      <c r="C1" s="99" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="59" t="s">
+      <c r="D1" s="99" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="61" t="s">
+      <c r="E1" s="101" t="s">
         <v>87</v>
       </c>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61" t="s">
+      <c r="F1" s="101"/>
+      <c r="G1" s="101"/>
+      <c r="H1" s="101" t="s">
         <v>89</v>
       </c>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
+      <c r="I1" s="101"/>
+      <c r="J1" s="101"/>
     </row>
     <row r="2" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="60"/>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
+      <c r="A2" s="100"/>
+      <c r="B2" s="100"/>
+      <c r="C2" s="100"/>
+      <c r="D2" s="100"/>
       <c r="E2" s="39" t="s">
         <v>90</v>
       </c>
@@ -3933,7 +3945,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView zoomScale="135" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="G17" sqref="A1:G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4257,16 +4269,16 @@
         <v>66</v>
       </c>
       <c r="D14" s="50">
-        <v>-5.55</v>
+        <v>-5.09</v>
       </c>
       <c r="E14" s="50" t="s">
         <v>69</v>
       </c>
       <c r="F14" s="50">
-        <v>-5.883</v>
+        <v>-5.4509999999999996</v>
       </c>
       <c r="G14" s="49" t="s">
-        <v>95</v>
+        <v>182</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -4280,16 +4292,16 @@
         <v>105</v>
       </c>
       <c r="D15" s="52">
-        <v>2.5089999999999999</v>
-      </c>
-      <c r="E15" s="52">
-        <v>1.2E-2</v>
+        <v>2.2069999999999999</v>
+      </c>
+      <c r="E15" s="51">
+        <v>2.7E-2</v>
       </c>
       <c r="F15" s="52">
-        <v>1.3440000000000001</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="G15" s="51" t="s">
-        <v>96</v>
+        <v>183</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -4303,16 +4315,16 @@
         <v>70</v>
       </c>
       <c r="D16" s="49">
-        <v>-0.91700000000000004</v>
+        <v>-1.3460000000000001</v>
       </c>
       <c r="E16" s="49">
-        <v>0.35899999999999999</v>
+        <v>0.17799999999999999</v>
       </c>
       <c r="F16" s="49">
-        <v>-5.5E-2</v>
+        <v>-7.8E-2</v>
       </c>
       <c r="G16" s="49" t="s">
-        <v>97</v>
+        <v>184</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -4326,16 +4338,16 @@
         <v>104</v>
       </c>
       <c r="D17" s="54">
-        <v>0.109</v>
-      </c>
-      <c r="E17" s="54">
-        <v>0.91300000000000003</v>
+        <v>0.54900000000000004</v>
+      </c>
+      <c r="E17" s="53">
+        <v>0.58299999999999996</v>
       </c>
       <c r="F17" s="54">
-        <v>4.0000000000000001E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="G17" s="53" t="s">
-        <v>98</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -4347,8 +4359,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6C21A91-93E6-A348-AEDB-74A761308800}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>